<commit_message>
Modified 08/08/2024 10:50:18 AM IST
</commit_message>
<xml_diff>
--- a/Extracted Data/VRU Headform (UC-C) - Color-wise Data & Graphs/2022_cars_combined.xlsx
+++ b/Extracted Data/VRU Headform (UC-C) - Color-wise Data & Graphs/2022_cars_combined.xlsx
@@ -8,7 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Graphs" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -135,1550 +134,6 @@
     </indexedColors>
   </colors>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="13"/>
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Default green</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <scatterChart>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <v>Default green</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <xVal>
-            <numRef>
-              <f>'Graphs'!$A$2:$A$64</f>
-            </numRef>
-          </xVal>
-          <yVal>
-            <numRef>
-              <f>'Graphs'!$B$2:$B$64</f>
-            </numRef>
-          </yVal>
-        </ser>
-        <ser>
-          <idx val="1"/>
-          <order val="1"/>
-          <tx>
-            <v>Average: 2.78</v>
-          </tx>
-          <spPr>
-            <a:ln w="30000">
-              <a:solidFill>
-                <a:srgbClr val="FFA500"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <xVal>
-            <numRef>
-              <f>'Graphs'!$A$2:$A$64</f>
-            </numRef>
-          </xVal>
-          <yVal>
-            <numRef>
-              <f>'Graphs'!$B$2:$B$64</f>
-            </numRef>
-          </yVal>
-        </ser>
-        <axId val="10"/>
-        <axId val="20"/>
-      </scatterChart>
-      <valAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Car Names</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="20"/>
-      </valAx>
-      <valAx>
-        <axId val="20"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>%-age</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="13"/>
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Green</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <scatterChart>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <v>Green</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <xVal>
-            <numRef>
-              <f>'Graphs'!$A$2:$A$64</f>
-            </numRef>
-          </xVal>
-          <yVal>
-            <numRef>
-              <f>'Graphs'!$C$2:$C$64</f>
-            </numRef>
-          </yVal>
-        </ser>
-        <ser>
-          <idx val="1"/>
-          <order val="1"/>
-          <tx>
-            <v>Average: 30.75</v>
-          </tx>
-          <spPr>
-            <a:ln w="30000">
-              <a:solidFill>
-                <a:srgbClr val="FFA500"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <xVal>
-            <numRef>
-              <f>'Graphs'!$A$2:$A$64</f>
-            </numRef>
-          </xVal>
-          <yVal>
-            <numRef>
-              <f>'Graphs'!$C$2:$C$64</f>
-            </numRef>
-          </yVal>
-        </ser>
-        <axId val="10"/>
-        <axId val="20"/>
-      </scatterChart>
-      <valAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Car Names</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="20"/>
-      </valAx>
-      <valAx>
-        <axId val="20"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>%-age</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="13"/>
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Yellow</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <scatterChart>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <v>Yellow</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <xVal>
-            <numRef>
-              <f>'Graphs'!$A$2:$A$64</f>
-            </numRef>
-          </xVal>
-          <yVal>
-            <numRef>
-              <f>'Graphs'!$D$2:$D$64</f>
-            </numRef>
-          </yVal>
-        </ser>
-        <ser>
-          <idx val="1"/>
-          <order val="1"/>
-          <tx>
-            <v>Average: 30.11</v>
-          </tx>
-          <spPr>
-            <a:ln w="30000">
-              <a:solidFill>
-                <a:srgbClr val="FFA500"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <xVal>
-            <numRef>
-              <f>'Graphs'!$A$2:$A$64</f>
-            </numRef>
-          </xVal>
-          <yVal>
-            <numRef>
-              <f>'Graphs'!$D$2:$D$64</f>
-            </numRef>
-          </yVal>
-        </ser>
-        <axId val="10"/>
-        <axId val="20"/>
-      </scatterChart>
-      <valAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Car Names</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="20"/>
-      </valAx>
-      <valAx>
-        <axId val="20"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>%-age</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="13"/>
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Orange</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <scatterChart>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <v>Orange</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <xVal>
-            <numRef>
-              <f>'Graphs'!$A$2:$A$64</f>
-            </numRef>
-          </xVal>
-          <yVal>
-            <numRef>
-              <f>'Graphs'!$E$2:$E$64</f>
-            </numRef>
-          </yVal>
-        </ser>
-        <ser>
-          <idx val="1"/>
-          <order val="1"/>
-          <tx>
-            <v>Average: 15.98</v>
-          </tx>
-          <spPr>
-            <a:ln w="30000">
-              <a:solidFill>
-                <a:srgbClr val="FFA500"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <xVal>
-            <numRef>
-              <f>'Graphs'!$A$2:$A$64</f>
-            </numRef>
-          </xVal>
-          <yVal>
-            <numRef>
-              <f>'Graphs'!$E$2:$E$64</f>
-            </numRef>
-          </yVal>
-        </ser>
-        <axId val="10"/>
-        <axId val="20"/>
-      </scatterChart>
-      <valAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Car Names</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="20"/>
-      </valAx>
-      <valAx>
-        <axId val="20"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>%-age</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="13"/>
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Brown</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <scatterChart>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <v>Brown</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <xVal>
-            <numRef>
-              <f>'Graphs'!$A$2:$A$64</f>
-            </numRef>
-          </xVal>
-          <yVal>
-            <numRef>
-              <f>'Graphs'!$F$2:$F$64</f>
-            </numRef>
-          </yVal>
-        </ser>
-        <ser>
-          <idx val="1"/>
-          <order val="1"/>
-          <tx>
-            <v>Average: 6.66</v>
-          </tx>
-          <spPr>
-            <a:ln w="30000">
-              <a:solidFill>
-                <a:srgbClr val="FFA500"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <xVal>
-            <numRef>
-              <f>'Graphs'!$A$2:$A$64</f>
-            </numRef>
-          </xVal>
-          <yVal>
-            <numRef>
-              <f>'Graphs'!$F$2:$F$64</f>
-            </numRef>
-          </yVal>
-        </ser>
-        <axId val="10"/>
-        <axId val="20"/>
-      </scatterChart>
-      <valAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Car Names</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="20"/>
-      </valAx>
-      <valAx>
-        <axId val="20"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>%-age</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="13"/>
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Red</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <scatterChart>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <v>Red</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <xVal>
-            <numRef>
-              <f>'Graphs'!$A$2:$A$64</f>
-            </numRef>
-          </xVal>
-          <yVal>
-            <numRef>
-              <f>'Graphs'!$G$2:$G$64</f>
-            </numRef>
-          </yVal>
-        </ser>
-        <ser>
-          <idx val="1"/>
-          <order val="1"/>
-          <tx>
-            <v>Average: 10.80</v>
-          </tx>
-          <spPr>
-            <a:ln w="30000">
-              <a:solidFill>
-                <a:srgbClr val="FFA500"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <xVal>
-            <numRef>
-              <f>'Graphs'!$A$2:$A$64</f>
-            </numRef>
-          </xVal>
-          <yVal>
-            <numRef>
-              <f>'Graphs'!$G$2:$G$64</f>
-            </numRef>
-          </yVal>
-        </ser>
-        <axId val="10"/>
-        <axId val="20"/>
-      </scatterChart>
-      <valAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Car Names</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="20"/>
-      </valAx>
-      <valAx>
-        <axId val="20"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>%-age</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="13"/>
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Default Red</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <scatterChart>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <v>Default Red</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <xVal>
-            <numRef>
-              <f>'Graphs'!$A$2:$A$64</f>
-            </numRef>
-          </xVal>
-          <yVal>
-            <numRef>
-              <f>'Graphs'!$H$2:$H$64</f>
-            </numRef>
-          </yVal>
-        </ser>
-        <ser>
-          <idx val="1"/>
-          <order val="1"/>
-          <tx>
-            <v>Average: 2.92</v>
-          </tx>
-          <spPr>
-            <a:ln w="30000">
-              <a:solidFill>
-                <a:srgbClr val="FFA500"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <xVal>
-            <numRef>
-              <f>'Graphs'!$A$2:$A$64</f>
-            </numRef>
-          </xVal>
-          <yVal>
-            <numRef>
-              <f>'Graphs'!$H$2:$H$64</f>
-            </numRef>
-          </yVal>
-        </ser>
-        <axId val="10"/>
-        <axId val="20"/>
-      </scatterChart>
-      <valAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Car Names</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="20"/>
-      </valAx>
-      <valAx>
-        <axId val="20"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>%-age</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="13"/>
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Blue</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <scatterChart>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <v>Blue</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <xVal>
-            <numRef>
-              <f>'Graphs'!$A$2:$A$64</f>
-            </numRef>
-          </xVal>
-          <yVal>
-            <numRef>
-              <f>'Graphs'!$I$2:$I$64</f>
-            </numRef>
-          </yVal>
-        </ser>
-        <ser>
-          <idx val="1"/>
-          <order val="1"/>
-          <tx>
-            <v>Average: 0.00</v>
-          </tx>
-          <spPr>
-            <a:ln w="30000">
-              <a:solidFill>
-                <a:srgbClr val="FFA500"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <xVal>
-            <numRef>
-              <f>'Graphs'!$A$2:$A$64</f>
-            </numRef>
-          </xVal>
-          <yVal>
-            <numRef>
-              <f>'Graphs'!$I$2:$I$64</f>
-            </numRef>
-          </yVal>
-        </ser>
-        <axId val="10"/>
-        <axId val="20"/>
-      </scatterChart>
-      <valAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Car Names</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="20"/>
-      </valAx>
-      <valAx>
-        <axId val="20"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>%-age</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="13"/>
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Predicted headform score (excluding blue points)</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <scatterChart>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <v>Predicted headform score (excluding blue points)</v>
-          </tx>
-          <spPr>
-            <a:ln>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <xVal>
-            <numRef>
-              <f>'Graphs'!$A$2:$A$64</f>
-            </numRef>
-          </xVal>
-          <yVal>
-            <numRef>
-              <f>'Graphs'!$J$2:$J$64</f>
-            </numRef>
-          </yVal>
-        </ser>
-        <ser>
-          <idx val="1"/>
-          <order val="1"/>
-          <tx>
-            <v>Average: 100.00</v>
-          </tx>
-          <spPr>
-            <a:ln w="30000">
-              <a:solidFill>
-                <a:srgbClr val="FFA500"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="none"/>
-            <spPr>
-              <a:ln>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <xVal>
-            <numRef>
-              <f>'Graphs'!$A$2:$A$64</f>
-            </numRef>
-          </xVal>
-          <yVal>
-            <numRef>
-              <f>'Graphs'!$J$2:$J$64</f>
-            </numRef>
-          </yVal>
-        </ser>
-        <axId val="10"/>
-        <axId val="20"/>
-      </scatterChart>
-      <valAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Car Names</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="20"/>
-      </valAx>
-      <valAx>
-        <axId val="20"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>%-age</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>0</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="2700000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="1" name="Chart 1"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>15</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="2700000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="2" name="Chart 2"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>30</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="2700000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="3" name="Chart 3"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>45</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="2700000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="4" name="Chart 4"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId4"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>60</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="2700000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="5" name="Chart 5"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId5"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>75</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="2700000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="6" name="Chart 6"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId6"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>90</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="2700000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="7" name="Chart 7"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId7"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>105</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="2700000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="8" name="Chart 8"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId8"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>120</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="2700000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="9" name="Chart 9"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart r:id="rId9"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4187,23 +2642,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Modified 08/08/2024 11:20:18 AM IST
</commit_message>
<xml_diff>
--- a/Extracted Data/VRU Headform (UC-C) - Color-wise Data & Graphs/2022_cars_combined.xlsx
+++ b/Extracted Data/VRU Headform (UC-C) - Color-wise Data & Graphs/2022_cars_combined.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Charts" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -134,6 +135,3413 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="13"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Default green</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <scatterChart>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>Series 1</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$B$1:$B$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <v>Series 2</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$C$1:$C$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="2"/>
+          <order val="2"/>
+          <tx>
+            <v>Series 3</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$D$1:$D$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="3"/>
+          <order val="3"/>
+          <tx>
+            <v>Series 4</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$E$1:$E$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="4"/>
+          <order val="4"/>
+          <tx>
+            <v>Series 5</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$F$1:$F$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="5"/>
+          <order val="5"/>
+          <tx>
+            <v>Series 6</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$G$1:$G$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="6"/>
+          <order val="6"/>
+          <tx>
+            <v>Series 7</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$H$1:$H$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="7"/>
+          <order val="7"/>
+          <tx>
+            <v>Series 8</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$I$1:$I$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="8"/>
+          <order val="8"/>
+          <tx>
+            <v>Series 9</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$J$1:$J$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <axId val="10"/>
+        <axId val="20"/>
+      </scatterChart>
+      <valAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Car Names</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="20"/>
+      </valAx>
+      <valAx>
+        <axId val="20"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Default green</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="13"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Green</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <scatterChart>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>Series 1</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$B$1:$B$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <v>Series 2</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$C$1:$C$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="2"/>
+          <order val="2"/>
+          <tx>
+            <v>Series 3</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$D$1:$D$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="3"/>
+          <order val="3"/>
+          <tx>
+            <v>Series 4</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$E$1:$E$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="4"/>
+          <order val="4"/>
+          <tx>
+            <v>Series 5</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$F$1:$F$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="5"/>
+          <order val="5"/>
+          <tx>
+            <v>Series 6</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$G$1:$G$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="6"/>
+          <order val="6"/>
+          <tx>
+            <v>Series 7</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$H$1:$H$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="7"/>
+          <order val="7"/>
+          <tx>
+            <v>Series 8</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$I$1:$I$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="8"/>
+          <order val="8"/>
+          <tx>
+            <v>Series 9</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$J$1:$J$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <axId val="10"/>
+        <axId val="20"/>
+      </scatterChart>
+      <valAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Car Names</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="20"/>
+      </valAx>
+      <valAx>
+        <axId val="20"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Green</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="13"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Yellow</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <scatterChart>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>Series 1</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$B$1:$B$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <v>Series 2</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$C$1:$C$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="2"/>
+          <order val="2"/>
+          <tx>
+            <v>Series 3</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$D$1:$D$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="3"/>
+          <order val="3"/>
+          <tx>
+            <v>Series 4</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$E$1:$E$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="4"/>
+          <order val="4"/>
+          <tx>
+            <v>Series 5</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$F$1:$F$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="5"/>
+          <order val="5"/>
+          <tx>
+            <v>Series 6</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$G$1:$G$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="6"/>
+          <order val="6"/>
+          <tx>
+            <v>Series 7</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$H$1:$H$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="7"/>
+          <order val="7"/>
+          <tx>
+            <v>Series 8</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$I$1:$I$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="8"/>
+          <order val="8"/>
+          <tx>
+            <v>Series 9</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$J$1:$J$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <axId val="10"/>
+        <axId val="20"/>
+      </scatterChart>
+      <valAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Car Names</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="20"/>
+      </valAx>
+      <valAx>
+        <axId val="20"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Yellow</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="13"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Orange</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <scatterChart>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>Series 1</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$B$1:$B$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <v>Series 2</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$C$1:$C$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="2"/>
+          <order val="2"/>
+          <tx>
+            <v>Series 3</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$D$1:$D$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="3"/>
+          <order val="3"/>
+          <tx>
+            <v>Series 4</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$E$1:$E$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="4"/>
+          <order val="4"/>
+          <tx>
+            <v>Series 5</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$F$1:$F$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="5"/>
+          <order val="5"/>
+          <tx>
+            <v>Series 6</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$G$1:$G$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="6"/>
+          <order val="6"/>
+          <tx>
+            <v>Series 7</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$H$1:$H$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="7"/>
+          <order val="7"/>
+          <tx>
+            <v>Series 8</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$I$1:$I$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="8"/>
+          <order val="8"/>
+          <tx>
+            <v>Series 9</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$J$1:$J$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <axId val="10"/>
+        <axId val="20"/>
+      </scatterChart>
+      <valAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Car Names</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="20"/>
+      </valAx>
+      <valAx>
+        <axId val="20"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Orange</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="13"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Brown</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <scatterChart>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>Series 1</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$B$1:$B$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <v>Series 2</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$C$1:$C$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="2"/>
+          <order val="2"/>
+          <tx>
+            <v>Series 3</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$D$1:$D$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="3"/>
+          <order val="3"/>
+          <tx>
+            <v>Series 4</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$E$1:$E$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="4"/>
+          <order val="4"/>
+          <tx>
+            <v>Series 5</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$F$1:$F$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="5"/>
+          <order val="5"/>
+          <tx>
+            <v>Series 6</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$G$1:$G$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="6"/>
+          <order val="6"/>
+          <tx>
+            <v>Series 7</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$H$1:$H$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="7"/>
+          <order val="7"/>
+          <tx>
+            <v>Series 8</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$I$1:$I$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="8"/>
+          <order val="8"/>
+          <tx>
+            <v>Series 9</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$J$1:$J$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <axId val="10"/>
+        <axId val="20"/>
+      </scatterChart>
+      <valAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Car Names</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="20"/>
+      </valAx>
+      <valAx>
+        <axId val="20"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Brown</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="13"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Red</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <scatterChart>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>Series 1</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$B$1:$B$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <v>Series 2</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$C$1:$C$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="2"/>
+          <order val="2"/>
+          <tx>
+            <v>Series 3</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$D$1:$D$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="3"/>
+          <order val="3"/>
+          <tx>
+            <v>Series 4</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$E$1:$E$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="4"/>
+          <order val="4"/>
+          <tx>
+            <v>Series 5</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$F$1:$F$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="5"/>
+          <order val="5"/>
+          <tx>
+            <v>Series 6</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$G$1:$G$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="6"/>
+          <order val="6"/>
+          <tx>
+            <v>Series 7</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$H$1:$H$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="7"/>
+          <order val="7"/>
+          <tx>
+            <v>Series 8</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$I$1:$I$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="8"/>
+          <order val="8"/>
+          <tx>
+            <v>Series 9</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$J$1:$J$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <axId val="10"/>
+        <axId val="20"/>
+      </scatterChart>
+      <valAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Car Names</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="20"/>
+      </valAx>
+      <valAx>
+        <axId val="20"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Red</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="13"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Default Red</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <scatterChart>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>Series 1</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$B$1:$B$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <v>Series 2</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$C$1:$C$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="2"/>
+          <order val="2"/>
+          <tx>
+            <v>Series 3</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$D$1:$D$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="3"/>
+          <order val="3"/>
+          <tx>
+            <v>Series 4</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$E$1:$E$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="4"/>
+          <order val="4"/>
+          <tx>
+            <v>Series 5</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$F$1:$F$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="5"/>
+          <order val="5"/>
+          <tx>
+            <v>Series 6</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$G$1:$G$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="6"/>
+          <order val="6"/>
+          <tx>
+            <v>Series 7</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$H$1:$H$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="7"/>
+          <order val="7"/>
+          <tx>
+            <v>Series 8</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$I$1:$I$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="8"/>
+          <order val="8"/>
+          <tx>
+            <v>Series 9</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$J$1:$J$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <axId val="10"/>
+        <axId val="20"/>
+      </scatterChart>
+      <valAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Car Names</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="20"/>
+      </valAx>
+      <valAx>
+        <axId val="20"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Default Red</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="13"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Blue</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <scatterChart>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>Series 1</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$B$1:$B$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <v>Series 2</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$C$1:$C$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="2"/>
+          <order val="2"/>
+          <tx>
+            <v>Series 3</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$D$1:$D$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="3"/>
+          <order val="3"/>
+          <tx>
+            <v>Series 4</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$E$1:$E$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="4"/>
+          <order val="4"/>
+          <tx>
+            <v>Series 5</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$F$1:$F$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="5"/>
+          <order val="5"/>
+          <tx>
+            <v>Series 6</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$G$1:$G$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="6"/>
+          <order val="6"/>
+          <tx>
+            <v>Series 7</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$H$1:$H$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="7"/>
+          <order val="7"/>
+          <tx>
+            <v>Series 8</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$I$1:$I$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="8"/>
+          <order val="8"/>
+          <tx>
+            <v>Series 9</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$J$1:$J$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <axId val="10"/>
+        <axId val="20"/>
+      </scatterChart>
+      <valAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Car Names</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="20"/>
+      </valAx>
+      <valAx>
+        <axId val="20"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Blue</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="13"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Predicted headform score (excluding blue points)</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <scatterChart>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <v>Series 1</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$B$1:$B$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <v>Series 2</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$C$1:$C$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="2"/>
+          <order val="2"/>
+          <tx>
+            <v>Series 3</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$D$1:$D$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="3"/>
+          <order val="3"/>
+          <tx>
+            <v>Series 4</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$E$1:$E$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="4"/>
+          <order val="4"/>
+          <tx>
+            <v>Series 5</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$F$1:$F$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="5"/>
+          <order val="5"/>
+          <tx>
+            <v>Series 6</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$G$1:$G$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="6"/>
+          <order val="6"/>
+          <tx>
+            <v>Series 7</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$H$1:$H$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="7"/>
+          <order val="7"/>
+          <tx>
+            <v>Series 8</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$I$1:$I$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <ser>
+          <idx val="8"/>
+          <order val="8"/>
+          <tx>
+            <v>Series 9</v>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <marker>
+            <symbol val="none"/>
+            <spPr>
+              <a:ln>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </spPr>
+          </marker>
+          <xVal>
+            <numRef>
+              <f>'Charts'!$A$2:$A$64</f>
+            </numRef>
+          </xVal>
+          <yVal>
+            <numRef>
+              <f>'Charts'!$J$1:$J$64</f>
+            </numRef>
+          </yVal>
+        </ser>
+        <axId val="10"/>
+        <axId val="20"/>
+      </scatterChart>
+      <valAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Car Names</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="20"/>
+      </valAx>
+      <valAx>
+        <axId val="20"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <title>
+          <tx>
+            <rich>
+              <a:bodyPr/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:t>Predicted headform score (excluding blue points)</a:t>
+                </a:r>
+              </a:p>
+            </rich>
+          </tx>
+        </title>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="2" name="Chart 2"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="3" name="Chart 3"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="4" name="Chart 4"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="5" name="Chart 5"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="6" name="Chart 6"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId6"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="7" name="Chart 7"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="8" name="Chart 8"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId8"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>0</col>
+      <colOff>0</colOff>
+      <row>14</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="9" name="Chart 9"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId9"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2642,4 +6050,23 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>